<commit_message>
Added information from 20 bunnies build with 1 triangle per leaf to the rendering stats spreadsheet.
</commit_message>
<xml_diff>
--- a/Project2/RenderingStats.xlsx
+++ b/Project2/RenderingStats.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
   <si>
     <t>Total Render Time</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>42.7560 seconds</t>
+  </si>
+  <si>
+    <t>24.8650 seconds</t>
   </si>
 </sst>
 </file>
@@ -517,7 +520,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -525,7 +528,7 @@
     <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
@@ -826,21 +829,33 @@
       <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="B10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="3">
+        <v>2778041</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1389021</v>
+      </c>
       <c r="E10" s="3">
         <v>1</v>
       </c>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
+      <c r="F10" s="3">
+        <v>262144</v>
+      </c>
+      <c r="G10" s="3">
+        <v>11156027</v>
+      </c>
       <c r="H10" s="3">
         <v>543772</v>
       </c>
       <c r="I10" s="3">
         <v>2.0743</v>
       </c>
-      <c r="J10" s="3"/>
+      <c r="J10" s="3">
+        <v>42.556899999999999</v>
+      </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="3" t="s">

</xml_diff>

<commit_message>
Formatted rendering stats and created pdf document for turnin.
</commit_message>
<xml_diff>
--- a/Project2/RenderingStats.xlsx
+++ b/Project2/RenderingStats.xlsx
@@ -137,7 +137,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -146,18 +146,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <fgColor theme="0" tint="-0.24994659260841701"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -208,21 +220,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -517,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -537,7 +589,7 @@
     <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="60.75" thickBot="1">
+    <row r="1" spans="1:10" s="8" customFormat="1" ht="60.75" thickBot="1">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -569,71 +621,71 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickTop="1">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:10" s="2" customFormat="1" ht="15.75" thickTop="1">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="1">
         <v>1153</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="1">
         <v>577</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="1">
         <v>1</v>
       </c>
-      <c r="F2" s="5">
-        <v>262144</v>
-      </c>
-      <c r="G2" s="5">
+      <c r="F2" s="1">
+        <v>262144</v>
+      </c>
+      <c r="G2" s="1">
         <v>2615720</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="1">
         <v>338699</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="1">
         <v>1.292</v>
       </c>
-      <c r="J2" s="5">
+      <c r="J2" s="1">
         <v>9.9781999999999993</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:10" s="5" customFormat="1">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="4">
         <v>669</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="4">
         <v>335</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="4">
         <v>2</v>
       </c>
-      <c r="F3" s="3">
-        <v>262144</v>
-      </c>
-      <c r="G3" s="3">
+      <c r="F3" s="4">
+        <v>262144</v>
+      </c>
+      <c r="G3" s="4">
         <v>2209412</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="4">
         <v>338699</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="4">
         <v>1.292</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J3" s="4">
         <v>8.4282000000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" s="2" customFormat="1">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -665,123 +717,103 @@
         <v>8.0716999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:10" s="10" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="9">
         <v>401</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="9">
         <v>201</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="9">
         <v>4</v>
       </c>
-      <c r="F5" s="3">
-        <v>262144</v>
-      </c>
-      <c r="G5" s="3">
+      <c r="F5" s="9">
+        <v>262144</v>
+      </c>
+      <c r="G5" s="9">
         <v>1990260</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="9">
         <v>338699</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="9">
         <v>1.292</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="9">
         <v>7.5922000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="2" customFormat="1">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:10" s="12" customFormat="1" ht="7.5" customHeight="1">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+    </row>
+    <row r="7" spans="1:10" s="2" customFormat="1">
+      <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C7" s="1">
         <v>138903</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D7" s="1">
         <v>69452</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E7" s="1">
         <v>1</v>
       </c>
-      <c r="F6" s="4">
-        <v>262144</v>
-      </c>
-      <c r="G6" s="4">
+      <c r="F7" s="1">
+        <v>262144</v>
+      </c>
+      <c r="G7" s="1">
         <v>759480</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H7" s="1">
         <v>233292</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I7" s="1">
         <v>0.88990000000000002</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J7" s="1">
         <v>2.8972000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="2" customFormat="1">
-      <c r="A7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="4">
-        <v>75963</v>
-      </c>
-      <c r="D7" s="4">
-        <v>37982</v>
-      </c>
-      <c r="E7" s="4">
-        <v>2</v>
-      </c>
-      <c r="F7" s="4">
-        <v>262144</v>
-      </c>
-      <c r="G7" s="4">
-        <v>728200</v>
-      </c>
-      <c r="H7" s="4">
-        <v>233292</v>
-      </c>
-      <c r="I7" s="4">
-        <v>0.88990000000000002</v>
-      </c>
-      <c r="J7" s="4">
-        <v>2.7778999999999998</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" s="2" customFormat="1">
+    <row r="8" spans="1:10" s="5" customFormat="1">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" s="4">
-        <v>63523</v>
+        <v>75963</v>
       </c>
       <c r="D8" s="4">
-        <v>31762</v>
+        <v>37982</v>
       </c>
       <c r="E8" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F8" s="4">
         <v>262144</v>
       </c>
       <c r="G8" s="4">
-        <v>721118</v>
+        <v>728200</v>
       </c>
       <c r="H8" s="4">
         <v>233292</v>
@@ -790,300 +822,362 @@
         <v>0.88990000000000002</v>
       </c>
       <c r="J8" s="4">
+        <v>2.7778999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="2" customFormat="1">
+      <c r="A9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="3">
+        <v>63523</v>
+      </c>
+      <c r="D9" s="3">
+        <v>31762</v>
+      </c>
+      <c r="E9" s="3">
+        <v>3</v>
+      </c>
+      <c r="F9" s="3">
+        <v>262144</v>
+      </c>
+      <c r="G9" s="3">
+        <v>721118</v>
+      </c>
+      <c r="H9" s="3">
+        <v>233292</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0.88990000000000002</v>
+      </c>
+      <c r="J9" s="3">
         <v>2.75</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="2" customFormat="1">
-      <c r="A9" s="4" t="s">
+    <row r="10" spans="1:10" s="10" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A10" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B10" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C10" s="9">
         <v>42693</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D10" s="9">
         <v>21347</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E10" s="9">
         <v>4</v>
       </c>
-      <c r="F9" s="4">
-        <v>262144</v>
-      </c>
-      <c r="G9" s="4">
+      <c r="F10" s="9">
+        <v>262144</v>
+      </c>
+      <c r="G10" s="9">
         <v>708572</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H10" s="9">
         <v>233292</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I10" s="9">
         <v>0.88990000000000002</v>
       </c>
-      <c r="J9" s="4">
+      <c r="J10" s="9">
         <v>2.7029999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="3" t="s">
+    <row r="11" spans="1:10" s="12" customFormat="1" ht="7.5" customHeight="1">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+    </row>
+    <row r="12" spans="1:10" s="2" customFormat="1">
+      <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C12" s="1">
         <v>2778041</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D12" s="1">
         <v>1389021</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E12" s="1">
         <v>1</v>
       </c>
-      <c r="F10" s="3">
-        <v>262144</v>
-      </c>
-      <c r="G10" s="3">
+      <c r="F12" s="1">
+        <v>262144</v>
+      </c>
+      <c r="G12" s="1">
         <v>11156027</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H12" s="1">
         <v>543772</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I12" s="1">
         <v>2.0743</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J12" s="1">
         <v>42.556899999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="3" t="s">
+    <row r="13" spans="1:10" s="5" customFormat="1">
+      <c r="A13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C13" s="4">
         <v>1551749</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D13" s="4">
         <v>775875</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E13" s="4">
         <v>2</v>
       </c>
-      <c r="F11" s="3">
-        <v>262144</v>
-      </c>
-      <c r="G11" s="3">
+      <c r="F13" s="4">
+        <v>262144</v>
+      </c>
+      <c r="G13" s="4">
         <v>10157778</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H13" s="4">
         <v>543772</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I13" s="4">
         <v>2.0743</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J13" s="4">
         <v>38.748800000000003</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="3" t="s">
+    <row r="14" spans="1:10" s="2" customFormat="1">
+      <c r="A14" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C14" s="3">
         <v>1245339</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D14" s="3">
         <v>622670</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E14" s="3">
         <v>3</v>
       </c>
-      <c r="F12" s="3">
-        <v>262144</v>
-      </c>
-      <c r="G12" s="3">
+      <c r="F14" s="3">
+        <v>262144</v>
+      </c>
+      <c r="G14" s="3">
         <v>9869439</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H14" s="3">
         <v>543772</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I14" s="3">
         <v>2.0743</v>
       </c>
-      <c r="J12" s="3">
+      <c r="J14" s="3">
         <v>37.648899999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="3" t="s">
+    <row r="15" spans="1:10" s="10" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A15" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B15" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C15" s="9">
         <v>868433</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D15" s="9">
         <v>434217</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E15" s="9">
         <v>4</v>
       </c>
-      <c r="F13" s="3">
-        <v>262144</v>
-      </c>
-      <c r="G13" s="3">
+      <c r="F15" s="9">
+        <v>262144</v>
+      </c>
+      <c r="G15" s="9">
         <v>9493982</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H15" s="9">
         <v>543772</v>
       </c>
-      <c r="I13" s="3">
+      <c r="I15" s="9">
         <v>2.0743</v>
       </c>
-      <c r="J13" s="3">
+      <c r="J15" s="9">
         <v>36.216700000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="2" customFormat="1">
-      <c r="A14" s="4" t="s">
+    <row r="16" spans="1:10" s="12" customFormat="1" ht="7.5" customHeight="1">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+    </row>
+    <row r="17" spans="1:10" s="2" customFormat="1">
+      <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C17" s="1">
         <v>132907</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D17" s="1">
         <v>66454</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E17" s="1">
         <v>1</v>
       </c>
-      <c r="F14" s="4">
-        <v>262144</v>
-      </c>
-      <c r="G14" s="4">
+      <c r="F17" s="1">
+        <v>262144</v>
+      </c>
+      <c r="G17" s="1">
         <v>20633614</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H17" s="1">
         <v>988900</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I17" s="1">
         <v>3.7724000000000002</v>
       </c>
-      <c r="J14" s="4">
+      <c r="J17" s="1">
         <v>78.710999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="2" customFormat="1">
-      <c r="A15" s="4" t="s">
+    <row r="18" spans="1:10" s="5" customFormat="1">
+      <c r="A18" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B18" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C18" s="4">
         <v>75027</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D18" s="4">
         <v>37514</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E18" s="4">
         <v>2</v>
       </c>
-      <c r="F15" s="4">
-        <v>262144</v>
-      </c>
-      <c r="G15" s="4">
+      <c r="F18" s="4">
+        <v>262144</v>
+      </c>
+      <c r="G18" s="4">
         <v>17845377</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H18" s="4">
         <v>988900</v>
       </c>
-      <c r="I15" s="4">
+      <c r="I18" s="4">
         <v>3.7724000000000002</v>
       </c>
-      <c r="J15" s="4">
+      <c r="J18" s="4">
         <v>68.074700000000007</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="2" customFormat="1">
-      <c r="A16" s="4" t="s">
+    <row r="19" spans="1:10" s="2" customFormat="1">
+      <c r="A19" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C19" s="3">
         <v>62695</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D19" s="3">
         <v>31348</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E19" s="3">
         <v>3</v>
       </c>
-      <c r="F16" s="4">
-        <v>262144</v>
-      </c>
-      <c r="G16" s="4">
+      <c r="F19" s="3">
+        <v>262144</v>
+      </c>
+      <c r="G19" s="3">
         <v>17279727</v>
       </c>
-      <c r="H16" s="4">
+      <c r="H19" s="3">
         <v>988900</v>
       </c>
-      <c r="I16" s="4">
+      <c r="I19" s="3">
         <v>3.7724000000000002</v>
       </c>
-      <c r="J16" s="4">
+      <c r="J19" s="3">
         <v>65.916899999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="2" customFormat="1">
-      <c r="A17" s="4" t="s">
+    <row r="20" spans="1:10" s="10" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A20" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B20" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C20" s="9">
         <v>42535</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D20" s="9">
         <v>21268</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E20" s="9">
         <v>4</v>
       </c>
-      <c r="F17" s="4">
-        <v>262144</v>
-      </c>
-      <c r="G17" s="4">
+      <c r="F20" s="9">
+        <v>262144</v>
+      </c>
+      <c r="G20" s="9">
         <v>16348937</v>
       </c>
-      <c r="H17" s="4">
+      <c r="H20" s="9">
         <v>988900</v>
       </c>
-      <c r="I17" s="4">
+      <c r="I20" s="9">
         <v>3.7724000000000002</v>
       </c>
-      <c r="J17" s="4">
+      <c r="J20" s="9">
         <v>62.366199999999999</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader xml:space="preserve">&amp;C&amp;"-,Bold"
+CSE 168: Assignment 2 Rendering Statistics
+ &amp;RRachelle Fuhrer
+</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Fixed the rendering stats documents so the # of bounding volume and triangle intersections is accurate.
</commit_message>
<xml_diff>
--- a/Project2/RenderingStats.xlsx
+++ b/Project2/RenderingStats.xlsx
@@ -572,7 +572,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -641,16 +641,16 @@
         <v>262144</v>
       </c>
       <c r="G2" s="1">
-        <v>2615720</v>
+        <v>4140992</v>
       </c>
       <c r="H2" s="1">
-        <v>338699</v>
+        <v>676320</v>
       </c>
       <c r="I2" s="1">
-        <v>1.292</v>
+        <v>2.58</v>
       </c>
       <c r="J2" s="1">
-        <v>9.9781999999999993</v>
+        <v>15.7966</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="5" customFormat="1">
@@ -673,16 +673,16 @@
         <v>262144</v>
       </c>
       <c r="G3" s="4">
-        <v>2209412</v>
+        <v>3666632</v>
       </c>
       <c r="H3" s="4">
-        <v>338699</v>
+        <v>744372</v>
       </c>
       <c r="I3" s="4">
-        <v>1.292</v>
+        <v>2.8395999999999999</v>
       </c>
       <c r="J3" s="4">
-        <v>8.4282000000000004</v>
+        <v>13.9871</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="2" customFormat="1">
@@ -705,16 +705,16 @@
         <v>262144</v>
       </c>
       <c r="G4" s="3">
-        <v>2115944</v>
+        <v>3525992</v>
       </c>
       <c r="H4" s="3">
-        <v>338699</v>
+        <v>807801</v>
       </c>
       <c r="I4" s="3">
-        <v>1.292</v>
+        <v>3.0815000000000001</v>
       </c>
       <c r="J4" s="3">
-        <v>8.0716999999999999</v>
+        <v>13.4506</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="10" customFormat="1" ht="15.75" thickBot="1">
@@ -737,16 +737,16 @@
         <v>262144</v>
       </c>
       <c r="G5" s="9">
-        <v>1990260</v>
+        <v>3305336</v>
       </c>
       <c r="H5" s="9">
-        <v>338699</v>
+        <v>995187</v>
       </c>
       <c r="I5" s="9">
-        <v>1.292</v>
+        <v>3.7963</v>
       </c>
       <c r="J5" s="9">
-        <v>7.5922000000000001</v>
+        <v>12.6089</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="12" customFormat="1" ht="7.5" customHeight="1">
@@ -781,16 +781,16 @@
         <v>262144</v>
       </c>
       <c r="G7" s="1">
-        <v>759480</v>
+        <v>1268926</v>
       </c>
       <c r="H7" s="1">
-        <v>233292</v>
+        <v>256089</v>
       </c>
       <c r="I7" s="1">
-        <v>0.88990000000000002</v>
+        <v>0.97689999999999999</v>
       </c>
       <c r="J7" s="1">
-        <v>2.8972000000000002</v>
+        <v>4.8406000000000002</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="5" customFormat="1">
@@ -813,16 +813,16 @@
         <v>262144</v>
       </c>
       <c r="G8" s="4">
-        <v>728200</v>
+        <v>1230050</v>
       </c>
       <c r="H8" s="4">
-        <v>233292</v>
+        <v>263685</v>
       </c>
       <c r="I8" s="4">
-        <v>0.88990000000000002</v>
+        <v>1.0059</v>
       </c>
       <c r="J8" s="4">
-        <v>2.7778999999999998</v>
+        <v>4.6923000000000004</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="2" customFormat="1">
@@ -845,16 +845,16 @@
         <v>262144</v>
       </c>
       <c r="G9" s="3">
-        <v>721118</v>
+        <v>1217088</v>
       </c>
       <c r="H9" s="3">
-        <v>233292</v>
+        <v>271923</v>
       </c>
       <c r="I9" s="3">
-        <v>0.88990000000000002</v>
+        <v>1.0373000000000001</v>
       </c>
       <c r="J9" s="3">
-        <v>2.75</v>
+        <v>4.6428000000000003</v>
       </c>
     </row>
     <row r="10" spans="1:10" s="10" customFormat="1" ht="15.75" thickBot="1">
@@ -877,16 +877,16 @@
         <v>262144</v>
       </c>
       <c r="G10" s="9">
-        <v>708572</v>
+        <v>1192690</v>
       </c>
       <c r="H10" s="9">
-        <v>233292</v>
+        <v>295474</v>
       </c>
       <c r="I10" s="9">
-        <v>0.88990000000000002</v>
+        <v>1.1271</v>
       </c>
       <c r="J10" s="9">
-        <v>2.7029999999999998</v>
+        <v>4.5498000000000003</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="12" customFormat="1" ht="7.5" customHeight="1">
@@ -921,16 +921,16 @@
         <v>262144</v>
       </c>
       <c r="G12" s="1">
-        <v>11156027</v>
+        <v>19878280</v>
       </c>
       <c r="H12" s="1">
-        <v>543772</v>
+        <v>1347795</v>
       </c>
       <c r="I12" s="1">
-        <v>2.0743</v>
+        <v>5.1414</v>
       </c>
       <c r="J12" s="1">
-        <v>42.556899999999999</v>
+        <v>75.829599999999999</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="5" customFormat="1">
@@ -941,10 +941,10 @@
         <v>17</v>
       </c>
       <c r="C13" s="4">
-        <v>1551749</v>
+        <v>1551753</v>
       </c>
       <c r="D13" s="4">
-        <v>775875</v>
+        <v>775877</v>
       </c>
       <c r="E13" s="4">
         <v>2</v>
@@ -953,16 +953,16 @@
         <v>262144</v>
       </c>
       <c r="G13" s="4">
-        <v>10157778</v>
+        <v>18615496</v>
       </c>
       <c r="H13" s="4">
-        <v>543772</v>
+        <v>1612530</v>
       </c>
       <c r="I13" s="4">
-        <v>2.0743</v>
+        <v>6.1513</v>
       </c>
       <c r="J13" s="4">
-        <v>38.748800000000003</v>
+        <v>71.012500000000003</v>
       </c>
     </row>
     <row r="14" spans="1:10" s="2" customFormat="1">
@@ -973,10 +973,10 @@
         <v>16</v>
       </c>
       <c r="C14" s="3">
-        <v>1245339</v>
+        <v>1245343</v>
       </c>
       <c r="D14" s="3">
-        <v>622670</v>
+        <v>622672</v>
       </c>
       <c r="E14" s="3">
         <v>3</v>
@@ -985,16 +985,16 @@
         <v>262144</v>
       </c>
       <c r="G14" s="3">
-        <v>9869439</v>
+        <v>18113938</v>
       </c>
       <c r="H14" s="3">
-        <v>543772</v>
+        <v>1908663</v>
       </c>
       <c r="I14" s="3">
-        <v>2.0743</v>
+        <v>7.2809999999999997</v>
       </c>
       <c r="J14" s="3">
-        <v>37.648899999999998</v>
+        <v>69.099199999999996</v>
       </c>
     </row>
     <row r="15" spans="1:10" s="10" customFormat="1" ht="15.75" thickBot="1">
@@ -1017,16 +1017,16 @@
         <v>262144</v>
       </c>
       <c r="G15" s="9">
-        <v>9493982</v>
+        <v>17417504</v>
       </c>
       <c r="H15" s="9">
-        <v>543772</v>
+        <v>2544567</v>
       </c>
       <c r="I15" s="9">
-        <v>2.0743</v>
+        <v>9.7067999999999994</v>
       </c>
       <c r="J15" s="9">
-        <v>36.216700000000003</v>
+        <v>66.442499999999995</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="12" customFormat="1" ht="7.5" customHeight="1">
@@ -1061,16 +1061,16 @@
         <v>262144</v>
       </c>
       <c r="G17" s="1">
-        <v>20633614</v>
+        <v>35167778</v>
       </c>
       <c r="H17" s="1">
-        <v>988900</v>
+        <v>3180800</v>
       </c>
       <c r="I17" s="1">
-        <v>3.7724000000000002</v>
+        <v>12.133800000000001</v>
       </c>
       <c r="J17" s="1">
-        <v>78.710999999999999</v>
+        <v>134.15440000000001</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="5" customFormat="1">
@@ -1093,16 +1093,16 @@
         <v>262144</v>
       </c>
       <c r="G18" s="4">
-        <v>17845377</v>
+        <v>32094392</v>
       </c>
       <c r="H18" s="4">
-        <v>988900</v>
+        <v>3465943</v>
       </c>
       <c r="I18" s="4">
-        <v>3.7724000000000002</v>
+        <v>13.221500000000001</v>
       </c>
       <c r="J18" s="4">
-        <v>68.074700000000007</v>
+        <v>122.43040000000001</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="2" customFormat="1">
@@ -1125,16 +1125,16 @@
         <v>262144</v>
       </c>
       <c r="G19" s="3">
-        <v>17279727</v>
+        <v>31282248</v>
       </c>
       <c r="H19" s="3">
-        <v>988900</v>
+        <v>3834671</v>
       </c>
       <c r="I19" s="3">
-        <v>3.7724000000000002</v>
+        <v>14.6281</v>
       </c>
       <c r="J19" s="3">
-        <v>65.916899999999998</v>
+        <v>119.3323</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="10" customFormat="1" ht="15.75" thickBot="1">
@@ -1157,16 +1157,16 @@
         <v>262144</v>
       </c>
       <c r="G20" s="9">
-        <v>16348937</v>
+        <v>29753636</v>
       </c>
       <c r="H20" s="9">
-        <v>988900</v>
+        <v>5020619</v>
       </c>
       <c r="I20" s="9">
-        <v>3.7724000000000002</v>
+        <v>19.152100000000001</v>
       </c>
       <c r="J20" s="9">
-        <v>62.366199999999999</v>
+        <v>113.50109999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>